<commit_message>
petit cangement dans le journal
</commit_message>
<xml_diff>
--- a/documentation/Lorenzo/3_1_Journal_Lorenzo.xlsx
+++ b/documentation/Lorenzo/3_1_Journal_Lorenzo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/lorenzo_magliani_studentfr_ch/Documents/Bureau/EMF/Documents EMF/Syntheses EMF/306/306-G3-SpeleoThink/documentation/Lorenzo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70311A96-1766-456A-9A75-DE2EF8160532}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61C3B1B1-E27C-43BF-9782-76D938221412}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>Insérer les lignes au-dessus de celle-ci !</t>
   </si>
@@ -69,9 +69,6 @@
       </rPr>
       <t>↓↓↓</t>
     </r>
-  </si>
-  <si>
-    <t>[no candidat]</t>
   </si>
   <si>
     <t>Total général &gt;</t>
@@ -1232,7 +1229,7 @@
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <pane ySplit="1" activePane="bottomLeft"/>
       <selection activeCell="A5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1246,7 +1243,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -1254,13 +1251,11 @@
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="28"/>
       <c r="C2" s="29"/>
-      <c r="D2" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="D2" s="4"/>
     </row>
     <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
@@ -1284,10 +1279,10 @@
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="36"/>
       <c r="D6" s="7">
@@ -1297,7 +1292,7 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="15"/>
       <c r="B7" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="8">
@@ -1307,7 +1302,7 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="15"/>
       <c r="B8" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="8">
@@ -1342,7 +1337,7 @@
     <row r="12" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15"/>
       <c r="B12" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="26"/>
@@ -1352,7 +1347,7 @@
         <v>46003</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="7">
@@ -1362,7 +1357,7 @@
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="15"/>
       <c r="B14" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="8">
@@ -1372,7 +1367,7 @@
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="15"/>
       <c r="B15" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="8">
@@ -1382,7 +1377,7 @@
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="15"/>
       <c r="B16" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="8">
@@ -1392,7 +1387,7 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="15"/>
       <c r="B17" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="8">
@@ -1402,7 +1397,7 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="15"/>
       <c r="B18" s="37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="8">
@@ -1425,7 +1420,7 @@
     <row r="20" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15"/>
       <c r="B20" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="26"/>
@@ -1875,7 +1870,7 @@
       <c r="A84" s="11"/>
       <c r="B84" s="10"/>
       <c r="C84" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D84" s="12">
         <f>D11+D19+D26+D33+D40+D47+D54+D61+D68+D75+D82</f>

</xml_diff>

<commit_message>
mise en place finale rover projet
</commit_message>
<xml_diff>
--- a/documentation/Lorenzo/3_1_Journal_Lorenzo.xlsx
+++ b/documentation/Lorenzo/3_1_Journal_Lorenzo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/lorenzo_magliani_studentfr_ch/Documents/Bureau/EMF/Documents EMF/Syntheses EMF/306/306-G3-SpeleoThink/documentation/Lorenzo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61C3B1B1-E27C-43BF-9782-76D938221412}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65047CD0-8762-4218-9F6A-5D40D564F003}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30750" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal_MAGLIANI_LORENZO" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>Insérer les lignes au-dessus de celle-ci !</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Total général &gt;</t>
-  </si>
-  <si>
-    <t>5.12.2025</t>
   </si>
   <si>
     <r>
@@ -141,6 +138,15 @@
   </si>
   <si>
     <t>J'ai rencontré un problème Majeur lors de la mise en place de l'application de test pour le rover et la manette, c'est pour cela que ça m'a pris autant de temps. Sinon dans la globalité de cette journée j'ai appris pas mal de choses et ça a été très utile pour mon développement professionnel</t>
+  </si>
+  <si>
+    <t>reprise en main du code mis en place la semaine précédente</t>
+  </si>
+  <si>
+    <t>C'était une journée plein de challenge, j'ai rencontré pas mal d'erreurs mais j'ai compris comment les résoudre.</t>
+  </si>
+  <si>
+    <t>intégration de java 17 au lieu de java 1.8 dans le projet</t>
   </si>
 </sst>
 </file>
@@ -486,108 +492,108 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1227,9 +1233,9 @@
   <dimension ref="A1:D85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" activePane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft"/>
       <selection activeCell="A5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1242,87 +1248,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-    </row>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="4"/>
     </row>
     <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="32"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="33"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="36"/>
+      <c r="A6" s="20">
+        <v>45996</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="23"/>
       <c r="D6" s="7">
         <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="20"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="25"/>
       <c r="D7" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="20"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="25"/>
       <c r="D8" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="25"/>
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1335,77 +1341,77 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
-      <c r="B12" s="24" t="s">
+      <c r="A12" s="21"/>
+      <c r="B12" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
+    </row>
+    <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="29">
+        <v>46003</v>
+      </c>
+      <c r="B13" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
-    </row>
-    <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14">
-        <v>46003</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="18"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
-      <c r="B14" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="20"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="25"/>
       <c r="D14" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
-      <c r="B15" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="20"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="25"/>
       <c r="D15" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="20"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="25"/>
       <c r="D16" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="20"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="25"/>
       <c r="D17" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
-      <c r="B18" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="38"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="33"/>
       <c r="D18" s="8">
         <v>1.5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="15"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
@@ -1418,45 +1424,51 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
-      <c r="B20" s="24" t="s">
+      <c r="A20" s="21"/>
+      <c r="B20" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="27"/>
+      <c r="D20" s="28"/>
+    </row>
+    <row r="21" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="29">
+        <v>46009</v>
+      </c>
+      <c r="B21" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="26"/>
-    </row>
-    <row r="21" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="7"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="7">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="15"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="25"/>
       <c r="D22" s="8"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="15"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="25"/>
       <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="15"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="25"/>
       <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="15"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="20"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="25"/>
       <c r="D25" s="8"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="15"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="2" t="s">
         <v>6</v>
       </c>
@@ -1465,47 +1477,55 @@
       </c>
       <c r="D26" s="9">
         <f>SUM(D21:D25)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="15"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="26"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="27"/>
+      <c r="D27" s="28"/>
     </row>
     <row r="28" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="7"/>
+      <c r="A28" s="29">
+        <v>46010</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="31"/>
+      <c r="D28" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="15"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="20"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="25"/>
       <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="15"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="20"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="25"/>
       <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="15"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="20"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="15"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="20"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="25"/>
       <c r="D32" s="8"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="15"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
@@ -1514,47 +1534,47 @@
       </c>
       <c r="D33" s="9">
         <f>SUM(D28:D32)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="16"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="23"/>
+      <c r="A34" s="34"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="37"/>
     </row>
     <row r="35" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="14"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="18"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="31"/>
       <c r="D35" s="7"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="15"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="20"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="25"/>
       <c r="D36" s="8"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="15"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="20"/>
+      <c r="A37" s="21"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="25"/>
       <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="15"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="20"/>
+      <c r="A38" s="21"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="25"/>
       <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="15"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="20"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="25"/>
       <c r="D39" s="8"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="15"/>
+      <c r="A40" s="21"/>
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
@@ -1567,43 +1587,43 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="16"/>
-      <c r="B41" s="21"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="23"/>
+      <c r="A41" s="34"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="37"/>
     </row>
     <row r="42" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="14"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="18"/>
+      <c r="A42" s="29"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="31"/>
       <c r="D42" s="7"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="15"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="20"/>
+      <c r="A43" s="21"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="25"/>
       <c r="D43" s="8"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="15"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="20"/>
+      <c r="A44" s="21"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="25"/>
       <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="15"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="20"/>
+      <c r="A45" s="21"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="25"/>
       <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="15"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="20"/>
+      <c r="A46" s="21"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="25"/>
       <c r="D46" s="8"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="15"/>
+      <c r="A47" s="21"/>
       <c r="B47" s="2" t="s">
         <v>6</v>
       </c>
@@ -1616,43 +1636,43 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="16"/>
-      <c r="B48" s="21"/>
-      <c r="C48" s="22"/>
-      <c r="D48" s="23"/>
+      <c r="A48" s="34"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="37"/>
     </row>
     <row r="49" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="14"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="18"/>
+      <c r="A49" s="29"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="31"/>
       <c r="D49" s="7"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="15"/>
-      <c r="B50" s="19"/>
-      <c r="C50" s="20"/>
+      <c r="A50" s="21"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="25"/>
       <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="15"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="20"/>
+      <c r="A51" s="21"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="25"/>
       <c r="D51" s="8"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="15"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="20"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="25"/>
       <c r="D52" s="8"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="15"/>
-      <c r="B53" s="19"/>
-      <c r="C53" s="20"/>
+      <c r="A53" s="21"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="25"/>
       <c r="D53" s="8"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="15"/>
+      <c r="A54" s="21"/>
       <c r="B54" s="2" t="s">
         <v>6</v>
       </c>
@@ -1665,43 +1685,43 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="16"/>
-      <c r="B55" s="21"/>
-      <c r="C55" s="22"/>
-      <c r="D55" s="23"/>
+      <c r="A55" s="34"/>
+      <c r="B55" s="35"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="37"/>
     </row>
     <row r="56" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="14"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="18"/>
+      <c r="A56" s="29"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="31"/>
       <c r="D56" s="7"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="15"/>
-      <c r="B57" s="19"/>
-      <c r="C57" s="20"/>
+      <c r="A57" s="21"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="25"/>
       <c r="D57" s="8"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="15"/>
-      <c r="B58" s="19"/>
-      <c r="C58" s="20"/>
+      <c r="A58" s="21"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="25"/>
       <c r="D58" s="8"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="15"/>
-      <c r="B59" s="19"/>
-      <c r="C59" s="20"/>
+      <c r="A59" s="21"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="25"/>
       <c r="D59" s="8"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="15"/>
-      <c r="B60" s="19"/>
-      <c r="C60" s="20"/>
+      <c r="A60" s="21"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="25"/>
       <c r="D60" s="8"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="15"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="2" t="s">
         <v>6</v>
       </c>
@@ -1714,43 +1734,43 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="16"/>
-      <c r="B62" s="21"/>
-      <c r="C62" s="22"/>
-      <c r="D62" s="23"/>
+      <c r="A62" s="34"/>
+      <c r="B62" s="35"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="37"/>
     </row>
     <row r="63" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="14"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="18"/>
+      <c r="A63" s="29"/>
+      <c r="B63" s="30"/>
+      <c r="C63" s="31"/>
       <c r="D63" s="7"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="15"/>
-      <c r="B64" s="19"/>
-      <c r="C64" s="20"/>
+      <c r="A64" s="21"/>
+      <c r="B64" s="24"/>
+      <c r="C64" s="25"/>
       <c r="D64" s="8"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="15"/>
-      <c r="B65" s="19"/>
-      <c r="C65" s="20"/>
+      <c r="A65" s="21"/>
+      <c r="B65" s="24"/>
+      <c r="C65" s="25"/>
       <c r="D65" s="8"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="15"/>
-      <c r="B66" s="19"/>
-      <c r="C66" s="20"/>
+      <c r="A66" s="21"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="25"/>
       <c r="D66" s="8"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="15"/>
-      <c r="B67" s="19"/>
-      <c r="C67" s="20"/>
+      <c r="A67" s="21"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="25"/>
       <c r="D67" s="8"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="15"/>
+      <c r="A68" s="21"/>
       <c r="B68" s="2" t="s">
         <v>6</v>
       </c>
@@ -1763,43 +1783,43 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="15"/>
-      <c r="B69" s="24"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="26"/>
+      <c r="A69" s="21"/>
+      <c r="B69" s="26"/>
+      <c r="C69" s="27"/>
+      <c r="D69" s="28"/>
     </row>
     <row r="70" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="14"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="18"/>
+      <c r="A70" s="29"/>
+      <c r="B70" s="30"/>
+      <c r="C70" s="31"/>
       <c r="D70" s="7"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="15"/>
-      <c r="B71" s="19"/>
-      <c r="C71" s="20"/>
+      <c r="A71" s="21"/>
+      <c r="B71" s="24"/>
+      <c r="C71" s="25"/>
       <c r="D71" s="8"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="15"/>
-      <c r="B72" s="19"/>
-      <c r="C72" s="20"/>
+      <c r="A72" s="21"/>
+      <c r="B72" s="24"/>
+      <c r="C72" s="25"/>
       <c r="D72" s="8"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="15"/>
-      <c r="B73" s="19"/>
-      <c r="C73" s="20"/>
+      <c r="A73" s="21"/>
+      <c r="B73" s="24"/>
+      <c r="C73" s="25"/>
       <c r="D73" s="8"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="15"/>
-      <c r="B74" s="19"/>
-      <c r="C74" s="20"/>
+      <c r="A74" s="21"/>
+      <c r="B74" s="24"/>
+      <c r="C74" s="25"/>
       <c r="D74" s="8"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="15"/>
+      <c r="A75" s="21"/>
       <c r="B75" s="2" t="s">
         <v>6</v>
       </c>
@@ -1812,43 +1832,43 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="16"/>
-      <c r="B76" s="21"/>
-      <c r="C76" s="22"/>
-      <c r="D76" s="23"/>
+      <c r="A76" s="34"/>
+      <c r="B76" s="35"/>
+      <c r="C76" s="36"/>
+      <c r="D76" s="37"/>
     </row>
     <row r="77" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="14"/>
-      <c r="B77" s="17"/>
-      <c r="C77" s="18"/>
+      <c r="A77" s="29"/>
+      <c r="B77" s="30"/>
+      <c r="C77" s="31"/>
       <c r="D77" s="7"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="15"/>
-      <c r="B78" s="19"/>
-      <c r="C78" s="20"/>
+      <c r="A78" s="21"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="25"/>
       <c r="D78" s="8"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="15"/>
-      <c r="B79" s="19"/>
-      <c r="C79" s="20"/>
+      <c r="A79" s="21"/>
+      <c r="B79" s="24"/>
+      <c r="C79" s="25"/>
       <c r="D79" s="8"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="15"/>
-      <c r="B80" s="19"/>
-      <c r="C80" s="20"/>
+      <c r="A80" s="21"/>
+      <c r="B80" s="24"/>
+      <c r="C80" s="25"/>
       <c r="D80" s="8"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="15"/>
-      <c r="B81" s="19"/>
-      <c r="C81" s="20"/>
+      <c r="A81" s="21"/>
+      <c r="B81" s="24"/>
+      <c r="C81" s="25"/>
       <c r="D81" s="8"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="15"/>
+      <c r="A82" s="21"/>
       <c r="B82" s="2" t="s">
         <v>6</v>
       </c>
@@ -1861,10 +1881,10 @@
       </c>
     </row>
     <row r="83" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="16"/>
-      <c r="B83" s="21"/>
-      <c r="C83" s="22"/>
-      <c r="D83" s="23"/>
+      <c r="A83" s="34"/>
+      <c r="B83" s="35"/>
+      <c r="C83" s="36"/>
+      <c r="D83" s="37"/>
     </row>
     <row r="84" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="11"/>
@@ -1874,19 +1894,91 @@
       </c>
       <c r="D84" s="12">
         <f>D11+D19+D26+D33+D40+D47+D54+D61+D68+D75+D82</f>
-        <v>10.5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="13" t="s">
+      <c r="A85" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B85" s="13"/>
-      <c r="C85" s="13"/>
-      <c r="D85" s="13"/>
+      <c r="B85" s="38"/>
+      <c r="C85" s="38"/>
+      <c r="D85" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="83">
+    <mergeCell ref="A85:D85"/>
+    <mergeCell ref="A77:A83"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="A63:A69"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="A49:A55"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="A42:A48"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="A35:A41"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="A28:A34"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="A13:A20"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B18:C18"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A4:A5"/>
@@ -1898,78 +1990,6 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A13:A20"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="A21:A27"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="A28:A34"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="A35:A41"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="A42:A48"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="A49:A55"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="A63:A69"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="A85:D85"/>
-    <mergeCell ref="A77:A83"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B83:D83"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D11">
     <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="Terminé">
@@ -2084,6 +2104,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BD0882D7B13D249A8B88997E24B9140" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="3865b25f2bf2a035dbe7787239b3f11c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8afaa137-8a18-4908-97f4-35fc924e5a91" xmlns:ns3="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="718f9f7ddd2530d56a17ab9424d0abda" ns2:_="" ns3:_="">
     <xsd:import namespace="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
@@ -2296,15 +2325,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2317,6 +2337,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84AEF82B-2BAE-481D-A319-B09ADD6915E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2335,14 +2363,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
   <ds:schemaRefs>

</xml_diff>